<commit_message>
Update Pipe Break Calculations.xlsx
Updated Pipe Break Calculations to be more visually appealing.
</commit_message>
<xml_diff>
--- a/surveys/Pipe Break Calculations.xlsx
+++ b/surveys/Pipe Break Calculations.xlsx
@@ -3,9 +3,9 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="20373"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DB146817-5666-44D7-9291-12E80486CD22}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABD0E6B1-44E2-43B0-B434-FB00485CA15A}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" activeTab="2" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" tabRatio="542" xr2:uid="{C50DDC91-227D-4C28-807B-6890084E472E}"/>
   </bookViews>
   <sheets>
     <sheet name="survey" sheetId="10" r:id="rId1"/>
@@ -56,7 +56,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2074" uniqueCount="1614">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2107" uniqueCount="1626">
   <si>
     <t>Question type</t>
   </si>
@@ -4815,9 +4815,6 @@
     <t>Date &amp; Time:</t>
   </si>
   <si>
-    <t>Pipe Break Inspection Form</t>
-  </si>
-  <si>
     <t>break_type</t>
   </si>
   <si>
@@ -4971,28 +4968,67 @@
     <t>no</t>
   </si>
   <si>
-    <t>image1</t>
-  </si>
-  <si>
     <t>Photo:</t>
   </si>
   <si>
-    <t>If you need to take a photo, do so here.</t>
-  </si>
-  <si>
-    <t>image2</t>
-  </si>
-  <si>
-    <t>image3</t>
-  </si>
-  <si>
     <t>Photos</t>
   </si>
   <si>
-    <t>https://services.arcgis.com/syn8rfJ2eTAK0T6k/arcgis/rest/services/Pipe_Break_Inspections/FeatureServer</t>
-  </si>
-  <si>
-    <t>Pipe Break Inspections</t>
+    <t>Water Loss Form</t>
+  </si>
+  <si>
+    <t>${Inspector}</t>
+  </si>
+  <si>
+    <t>w2</t>
+  </si>
+  <si>
+    <t>Please enter a pipe diameter.</t>
+  </si>
+  <si>
+    <t>Please enter the width of the break.</t>
+  </si>
+  <si>
+    <t>Please enter the pressure in PSI.</t>
+  </si>
+  <si>
+    <t>Please enter the leak time in minutes.</t>
+  </si>
+  <si>
+    <t>Ensure you've entered all data for the calculation.</t>
+  </si>
+  <si>
+    <t>Please enter the leak time.</t>
+  </si>
+  <si>
+    <t>numOfPhotos</t>
+  </si>
+  <si>
+    <t>Please choose the number of photos you are taking.</t>
+  </si>
+  <si>
+    <t>start=0, end=5, step=1</t>
+  </si>
+  <si>
+    <t>InspectionPhotos</t>
+  </si>
+  <si>
+    <t>Inspection Photos</t>
+  </si>
+  <si>
+    <t>${numOfPhotos}</t>
+  </si>
+  <si>
+    <t>InspectionPhoto</t>
+  </si>
+  <si>
+    <t>ProjectInfo</t>
+  </si>
+  <si>
+    <t>Project Information</t>
+  </si>
+  <si>
+    <t>grid w2</t>
   </si>
 </sst>
 </file>
@@ -5370,6 +5406,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
@@ -5379,7 +5416,6 @@
     <xf numFmtId="49" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
@@ -5791,7 +5827,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E8BCF28F-4446-420A-A249-4C129790FE67}" name="tblSurvey" displayName="tblSurvey" ref="A1:AN154" totalsRowShown="0" headerRowDxfId="23">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{E8BCF28F-4446-420A-A249-4C129790FE67}" name="tblSurvey" displayName="tblSurvey" ref="A1:AN158" totalsRowShown="0" headerRowDxfId="23">
   <tableColumns count="40">
     <tableColumn id="1" xr3:uid="{022962FC-8CC9-4AB6-B048-71E74C206995}" name="type"/>
     <tableColumn id="2" xr3:uid="{6DA5C753-F0F7-4FC1-B05D-B91AAB5BAB3F}" name="name"/>
@@ -6184,11 +6220,11 @@
   <sheetPr>
     <tabColor rgb="FF00B050"/>
   </sheetPr>
-  <dimension ref="A1:AN31"/>
+  <dimension ref="A1:AN35"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane xSplit="4" topLeftCell="E1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight" activeCell="F17" sqref="F17"/>
+      <selection pane="topRight" activeCell="I4" sqref="I4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6330,50 +6366,47 @@
     </row>
     <row r="2" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>27</v>
       </c>
       <c r="B2" t="s">
-        <v>1550</v>
+        <v>1623</v>
       </c>
       <c r="C2" t="s">
-        <v>1551</v>
-      </c>
-      <c r="T2" t="s">
-        <v>102</v>
+        <v>1624</v>
+      </c>
+      <c r="F2" t="s">
+        <v>1625</v>
       </c>
     </row>
     <row r="3" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>24</v>
+        <v>11</v>
       </c>
       <c r="B3" t="s">
-        <v>1552</v>
+        <v>1550</v>
       </c>
       <c r="C3" t="s">
-        <v>1553</v>
-      </c>
-      <c r="I3" t="s">
-        <v>114</v>
-      </c>
-      <c r="K3" t="s">
-        <v>117</v>
+        <v>1551</v>
       </c>
       <c r="T3" t="s">
-        <v>92</v>
+        <v>102</v>
       </c>
     </row>
     <row r="4" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>24</v>
       </c>
       <c r="B4" t="s">
-        <v>1597</v>
+        <v>1552</v>
       </c>
       <c r="C4" t="s">
-        <v>1598</v>
+        <v>1553</v>
+      </c>
+      <c r="K4" t="s">
+        <v>117</v>
       </c>
       <c r="T4" t="s">
-        <v>102</v>
+        <v>92</v>
       </c>
     </row>
     <row r="5" spans="1:40" x14ac:dyDescent="0.25">
@@ -6381,10 +6414,10 @@
         <v>11</v>
       </c>
       <c r="B5" t="s">
-        <v>1599</v>
+        <v>1596</v>
       </c>
       <c r="C5" t="s">
-        <v>1600</v>
+        <v>1597</v>
       </c>
       <c r="T5" t="s">
         <v>102</v>
@@ -6392,16 +6425,13 @@
     </row>
     <row r="6" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>1560</v>
+        <v>11</v>
       </c>
       <c r="B6" t="s">
-        <v>1561</v>
+        <v>1598</v>
       </c>
       <c r="C6" t="s">
-        <v>1562</v>
-      </c>
-      <c r="F6" t="s">
-        <v>79</v>
+        <v>1599</v>
       </c>
       <c r="T6" t="s">
         <v>102</v>
@@ -6409,104 +6439,84 @@
     </row>
     <row r="7" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>27</v>
+        <v>1559</v>
       </c>
       <c r="B7" t="s">
-        <v>1559</v>
+        <v>1560</v>
       </c>
       <c r="C7" t="s">
-        <v>1556</v>
-      </c>
-      <c r="N7" t="s">
-        <v>1584</v>
+        <v>1561</v>
+      </c>
+      <c r="F7" t="s">
+        <v>79</v>
+      </c>
+      <c r="T7" t="s">
+        <v>102</v>
       </c>
     </row>
     <row r="8" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>6</v>
-      </c>
-      <c r="B8" t="s">
-        <v>1563</v>
-      </c>
-      <c r="C8" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1592</v>
-      </c>
-      <c r="T8" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="9" spans="1:40" x14ac:dyDescent="0.25">
-      <c r="A9" t="s">
-        <v>6</v>
-      </c>
-      <c r="B9" t="s">
-        <v>1565</v>
-      </c>
-      <c r="C9" t="s">
-        <v>1566</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1592</v>
-      </c>
-      <c r="T9" t="s">
-        <v>96</v>
+        <v>29</v>
       </c>
     </row>
     <row r="10" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
-        <v>6</v>
+        <v>27</v>
       </c>
       <c r="B10" t="s">
-        <v>1567</v>
+        <v>1558</v>
       </c>
       <c r="C10" t="s">
-        <v>1568</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1569</v>
-      </c>
-      <c r="T10" t="s">
-        <v>96</v>
-      </c>
-    </row>
-    <row r="11" spans="1:40" ht="17.25" x14ac:dyDescent="0.25">
+        <v>1555</v>
+      </c>
+      <c r="F10" t="s">
+        <v>1609</v>
+      </c>
+      <c r="N10" t="s">
+        <v>1583</v>
+      </c>
+    </row>
+    <row r="11" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>6</v>
       </c>
       <c r="B11" t="s">
-        <v>1572</v>
+        <v>1562</v>
       </c>
       <c r="C11" t="s">
-        <v>1573</v>
+        <v>1563</v>
       </c>
       <c r="D11" t="s">
-        <v>1574</v>
+        <v>1591</v>
+      </c>
+      <c r="G11" t="s">
+        <v>114</v>
+      </c>
+      <c r="H11" t="s">
+        <v>1610</v>
       </c>
       <c r="T11" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="12" spans="1:40" ht="17.25" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:40" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
         <v>6</v>
       </c>
       <c r="B12" t="s">
-        <v>1577</v>
+        <v>1564</v>
       </c>
       <c r="C12" t="s">
-        <v>1570</v>
+        <v>1565</v>
       </c>
       <c r="D12" t="s">
-        <v>1571</v>
-      </c>
-      <c r="I12" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G12" t="s">
         <v>114</v>
       </c>
-      <c r="K12" t="s">
-        <v>1585</v>
+      <c r="H12" t="s">
+        <v>1611</v>
       </c>
       <c r="T12" t="s">
         <v>96</v>
@@ -6517,42 +6527,42 @@
         <v>6</v>
       </c>
       <c r="B13" t="s">
-        <v>1575</v>
+        <v>1566</v>
       </c>
       <c r="C13" t="s">
-        <v>1580</v>
+        <v>1567</v>
       </c>
       <c r="D13" t="s">
-        <v>1576</v>
-      </c>
-      <c r="I13" t="s">
+        <v>1568</v>
+      </c>
+      <c r="G13" t="s">
         <v>114</v>
       </c>
-      <c r="K13" t="s">
-        <v>1582</v>
+      <c r="H13" t="s">
+        <v>1612</v>
       </c>
       <c r="T13" t="s">
         <v>96</v>
       </c>
     </row>
-    <row r="14" spans="1:40" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:40" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
         <v>6</v>
       </c>
       <c r="B14" t="s">
-        <v>1578</v>
+        <v>1571</v>
       </c>
       <c r="C14" t="s">
-        <v>1579</v>
+        <v>1572</v>
       </c>
       <c r="D14" t="s">
-        <v>1581</v>
-      </c>
-      <c r="I14" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G14" t="s">
         <v>114</v>
       </c>
-      <c r="K14" t="s">
-        <v>1583</v>
+      <c r="H14" t="s">
+        <v>1613</v>
       </c>
       <c r="T14" t="s">
         <v>96</v>
@@ -6560,242 +6570,376 @@
     </row>
     <row r="15" spans="1:40" ht="17.25" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1576</v>
+      </c>
+      <c r="C15" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G15" t="s">
+        <v>114</v>
+      </c>
+      <c r="H15" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I15" t="s">
+        <v>114</v>
+      </c>
+      <c r="K15" t="s">
+        <v>1584</v>
+      </c>
+      <c r="T15" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="16" spans="1:40" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>1574</v>
+      </c>
+      <c r="C16" t="s">
+        <v>1579</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G16" t="s">
+        <v>114</v>
+      </c>
+      <c r="H16" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I16" t="s">
+        <v>114</v>
+      </c>
+      <c r="K16" t="s">
+        <v>1581</v>
+      </c>
+      <c r="T16" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="17" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>1577</v>
+      </c>
+      <c r="C17" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G17" t="s">
+        <v>114</v>
+      </c>
+      <c r="H17" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I17" t="s">
+        <v>114</v>
+      </c>
+      <c r="K17" t="s">
+        <v>1582</v>
+      </c>
+      <c r="T17" t="s">
+        <v>96</v>
+      </c>
+    </row>
+    <row r="18" spans="1:25" ht="17.25" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="16" spans="1:40" ht="17.25" x14ac:dyDescent="0.25"/>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
+    <row r="19" spans="1:25" ht="17.25" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A20" t="s">
         <v>27</v>
       </c>
-      <c r="B17" t="s">
+      <c r="B20" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C20" t="s">
         <v>1557</v>
       </c>
-      <c r="C17" t="s">
-        <v>1558</v>
-      </c>
-      <c r="N17" t="s">
-        <v>1591</v>
-      </c>
-    </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>6</v>
-      </c>
-      <c r="B18" t="s">
-        <v>1586</v>
-      </c>
-      <c r="C18" t="s">
-        <v>1564</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1592</v>
-      </c>
-    </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A19" t="s">
-        <v>6</v>
-      </c>
-      <c r="B19" t="s">
-        <v>1587</v>
-      </c>
-      <c r="C19" t="s">
-        <v>1568</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A20" t="s">
-        <v>6</v>
-      </c>
-      <c r="B20" t="s">
-        <v>1588</v>
-      </c>
-      <c r="C20" t="s">
-        <v>1573</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1574</v>
-      </c>
-    </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="F20" t="s">
+        <v>1609</v>
+      </c>
+      <c r="N20" t="s">
+        <v>1590</v>
+      </c>
+    </row>
+    <row r="21" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>1593</v>
+        <v>1585</v>
       </c>
       <c r="C21" t="s">
-        <v>1570</v>
+        <v>1563</v>
       </c>
       <c r="D21" t="s">
-        <v>1571</v>
-      </c>
-      <c r="I21" t="s">
+        <v>1591</v>
+      </c>
+      <c r="G21" t="s">
         <v>114</v>
       </c>
-      <c r="K21" t="s">
-        <v>1596</v>
-      </c>
-    </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H21" t="s">
+        <v>1610</v>
+      </c>
+    </row>
+    <row r="22" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>6</v>
       </c>
       <c r="B22" t="s">
-        <v>1589</v>
+        <v>1586</v>
       </c>
       <c r="C22" t="s">
-        <v>1580</v>
+        <v>1567</v>
       </c>
       <c r="D22" t="s">
-        <v>1576</v>
-      </c>
-      <c r="I22" t="s">
+        <v>1568</v>
+      </c>
+      <c r="G22" t="s">
         <v>114</v>
       </c>
-      <c r="K22" t="s">
-        <v>1594</v>
-      </c>
-    </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
+      <c r="H22" t="s">
+        <v>1612</v>
+      </c>
+    </row>
+    <row r="23" spans="1:25" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>6</v>
       </c>
       <c r="B23" t="s">
-        <v>1590</v>
+        <v>1587</v>
       </c>
       <c r="C23" t="s">
+        <v>1572</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1573</v>
+      </c>
+      <c r="G23" t="s">
+        <v>114</v>
+      </c>
+      <c r="H23" t="s">
+        <v>1615</v>
+      </c>
+    </row>
+    <row r="24" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A24" t="s">
+        <v>6</v>
+      </c>
+      <c r="B24" t="s">
+        <v>1592</v>
+      </c>
+      <c r="C24" t="s">
+        <v>1569</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1570</v>
+      </c>
+      <c r="G24" t="s">
+        <v>114</v>
+      </c>
+      <c r="H24" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I24" t="s">
+        <v>114</v>
+      </c>
+      <c r="K24" t="s">
+        <v>1595</v>
+      </c>
+    </row>
+    <row r="25" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A25" t="s">
+        <v>6</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1588</v>
+      </c>
+      <c r="C25" t="s">
         <v>1579</v>
       </c>
-      <c r="D23" t="s">
-        <v>1581</v>
-      </c>
-      <c r="I23" t="s">
+      <c r="D25" t="s">
+        <v>1575</v>
+      </c>
+      <c r="G25" t="s">
         <v>114</v>
       </c>
-      <c r="K23" t="s">
-        <v>1595</v>
-      </c>
-    </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A24" t="s">
+      <c r="H25" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I25" t="s">
+        <v>114</v>
+      </c>
+      <c r="K25" t="s">
+        <v>1593</v>
+      </c>
+    </row>
+    <row r="26" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A26" t="s">
+        <v>6</v>
+      </c>
+      <c r="B26" t="s">
+        <v>1589</v>
+      </c>
+      <c r="C26" t="s">
+        <v>1578</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1580</v>
+      </c>
+      <c r="G26" t="s">
+        <v>114</v>
+      </c>
+      <c r="H26" t="s">
+        <v>1614</v>
+      </c>
+      <c r="I26" t="s">
+        <v>114</v>
+      </c>
+      <c r="K26" t="s">
+        <v>1594</v>
+      </c>
+    </row>
+    <row r="27" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>29</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A26" t="s">
-        <v>1603</v>
-      </c>
-      <c r="B26" t="s">
+    <row r="29" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
+        <v>1602</v>
+      </c>
+      <c r="B29" t="s">
+        <v>1600</v>
+      </c>
+      <c r="C29" t="s">
         <v>1601</v>
       </c>
-      <c r="C26" t="s">
-        <v>1602</v>
-      </c>
-      <c r="F26" t="s">
+      <c r="F29" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+    <row r="30" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A30" t="s">
         <v>27</v>
       </c>
-      <c r="B27" t="s">
-        <v>1611</v>
-      </c>
-      <c r="C27" t="s">
-        <v>1611</v>
-      </c>
-      <c r="F27" t="s">
+      <c r="B30" t="s">
+        <v>1606</v>
+      </c>
+      <c r="C30" t="s">
+        <v>1606</v>
+      </c>
+      <c r="F30" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A28" t="s">
+    <row r="31" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1616</v>
+      </c>
+      <c r="C31" t="s">
+        <v>1617</v>
+      </c>
+      <c r="G31" t="s">
+        <v>114</v>
+      </c>
+      <c r="H31" t="s">
+        <v>1617</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>1618</v>
+      </c>
+    </row>
+    <row r="32" spans="1:25" x14ac:dyDescent="0.25">
+      <c r="A32" t="s">
+        <v>31</v>
+      </c>
+      <c r="B32" t="s">
+        <v>1619</v>
+      </c>
+      <c r="C32" t="s">
+        <v>1620</v>
+      </c>
+      <c r="P32" t="s">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="33" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A33" t="s">
         <v>26</v>
       </c>
-      <c r="B28" t="s">
-        <v>1606</v>
-      </c>
-      <c r="C28" t="s">
-        <v>1607</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>26</v>
-      </c>
-      <c r="B29" t="s">
-        <v>1609</v>
-      </c>
-      <c r="C29" t="s">
-        <v>1607</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A30" t="s">
-        <v>26</v>
-      </c>
-      <c r="B30" t="s">
-        <v>1610</v>
-      </c>
-      <c r="C30" t="s">
-        <v>1607</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1608</v>
-      </c>
-    </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B33" t="s">
+        <v>1622</v>
+      </c>
+      <c r="C33" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="34" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A34" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="35" spans="1:3" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
         <v>29</v>
       </c>
     </row>
   </sheetData>
   <dataConsolidate/>
   <phoneticPr fontId="12" type="noConversion"/>
-  <conditionalFormatting sqref="B15:B16">
+  <conditionalFormatting sqref="B18:B19">
     <cfRule type="duplicateValues" dxfId="9" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B13">
+  <conditionalFormatting sqref="B16">
     <cfRule type="duplicateValues" dxfId="8" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B12">
+  <conditionalFormatting sqref="B15">
     <cfRule type="duplicateValues" dxfId="7" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="B2:B11 B17:B154 B14">
-    <cfRule type="duplicateValues" dxfId="6" priority="13"/>
+  <conditionalFormatting sqref="B3:B14 B20:B158 B17">
+    <cfRule type="duplicateValues" dxfId="6" priority="14"/>
   </conditionalFormatting>
   <dataValidations count="7">
-    <dataValidation type="list" allowBlank="1" sqref="A2:A16 A18:A154" xr:uid="{5A5EBDF2-8D76-4B72-B739-2B3433DFC758}">
+    <dataValidation type="list" allowBlank="1" sqref="A21:A158 A3:A19" xr:uid="{5A5EBDF2-8D76-4B72-B739-2B3433DFC758}">
       <formula1>QuestionTypes</formula1>
     </dataValidation>
-    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Question names:_x000a__x000a_• Must be unique_x000a_• Must start with a letter_x000a_• Can only contain letters, numbers and underscores_x000a_• Cannot contain reserved keywords or special characters_x000a_• Cannot exceed 31 characters (ArcGIS Enterprise)" sqref="B2:B154" xr:uid="{AE52CDED-D21E-4469-BBC3-752225966B97}">
-      <formula1>AND(ISERR(LEFT(B2,1)*1),LEN(B2)=LEN(SUBSTITUTE(B2," ","")),LEN(B2)&lt;32,COUNTIF(Reserved,B2)=0,SUMPRODUCT(--ISNUMBER(SEARCH(SpecialChars,B2)))=0)</formula1>
+    <dataValidation type="custom" errorStyle="warning" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Name" error="Question names:_x000a__x000a_• Must be unique_x000a_• Must start with a letter_x000a_• Can only contain letters, numbers and underscores_x000a_• Cannot contain reserved keywords or special characters_x000a_• Cannot exceed 31 characters (ArcGIS Enterprise)" sqref="B3:B158" xr:uid="{AE52CDED-D21E-4469-BBC3-752225966B97}">
+      <formula1>AND(ISERR(LEFT(B3,1)*1),LEN(B3)=LEN(SUBSTITUTE(B3," ","")),LEN(B3)&lt;32,COUNTIF(Reserved,B3)=0,SUMPRODUCT(--ISNUMBER(SEARCH(SpecialChars,B3)))=0)</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="G2:G154 I2:I154" xr:uid="{DBB329AD-6667-4687-A562-56C9714BF775}">
+    <dataValidation type="list" allowBlank="1" sqref="I3:I158 G3:G158" xr:uid="{DBB329AD-6667-4687-A562-56C9714BF775}">
       <formula1>"yes"</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S2:S154" xr:uid="{79E6C9D0-5240-48E7-92BD-276D4F191BD2}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Bind Type" error="The value you have entered is not one of the supported bind types." sqref="S3:S158" xr:uid="{79E6C9D0-5240-48E7-92BD-276D4F191BD2}">
       <formula1>BindTypes</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T2:T154" xr:uid="{69D93EA3-D84F-4D6A-AEF4-4511EFBDF101}">
+    <dataValidation type="list" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Type" error="The value you have entered is not one of the supported field types." sqref="T3:T158" xr:uid="{69D93EA3-D84F-4D6A-AEF4-4511EFBDF101}">
       <formula1>EsriFieldTypes</formula1>
     </dataValidation>
-    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U2:U154" xr:uid="{42CD8278-AF02-4B5F-9715-CBA2F5F38143}">
+    <dataValidation type="whole" operator="greaterThan" allowBlank="1" showErrorMessage="1" errorTitle="Invalid Field Length" error="Please enter a whole number greater than zero." sqref="U3:U158" xr:uid="{42CD8278-AF02-4B5F-9715-CBA2F5F38143}">
       <formula1>0</formula1>
     </dataValidation>
-    <dataValidation type="list" allowBlank="1" sqref="F2:F154" xr:uid="{6CE37BE8-524C-4D34-948C-B68B9CD7C386}">
-      <formula1>IF(LEFT(A2,4)="rank",appearRank,IF(LEFT(A2,8)="select_m",appearSelMulti,IF(LEFT(A2,8)="select_o",appearSelOne,IF(A2="begin group",appearBeginGrp,IF(A2="begin repeat",appearBeginRpt,INDIRECT("appear"&amp;A2))))))</formula1>
+    <dataValidation type="list" allowBlank="1" sqref="F3:F158" xr:uid="{6CE37BE8-524C-4D34-948C-B68B9CD7C386}">
+      <formula1>IF(LEFT(A3,4)="rank",appearRank,IF(LEFT(A3,8)="select_m",appearSelMulti,IF(LEFT(A3,8)="select_o",appearSelOne,IF(A3="begin group",appearBeginGrp,IF(A3="begin repeat",appearBeginRpt,INDIRECT("appear"&amp;A3))))))</formula1>
     </dataValidation>
   </dataValidations>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -6852,29 +6996,29 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
+        <v>1554</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1558</v>
+      </c>
+      <c r="C2" t="s">
         <v>1555</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1559</v>
-      </c>
-      <c r="C2" t="s">
-        <v>1556</v>
       </c>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>1555</v>
+        <v>1554</v>
       </c>
       <c r="B3" t="s">
+        <v>1556</v>
+      </c>
+      <c r="C3" t="s">
         <v>1557</v>
-      </c>
-      <c r="C3" t="s">
-        <v>1558</v>
       </c>
     </row>
     <row r="5" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
       <c r="B5" t="s">
         <v>114</v>
@@ -6885,10 +7029,10 @@
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
+        <v>1603</v>
+      </c>
+      <c r="B6" t="s">
         <v>1604</v>
-      </c>
-      <c r="B6" t="s">
-        <v>1605</v>
       </c>
       <c r="C6" t="s">
         <v>10</v>
@@ -6907,8 +7051,8 @@
   </sheetPr>
   <dimension ref="A1:H2"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B24" sqref="B24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -6946,14 +7090,12 @@
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>1554</v>
-      </c>
-      <c r="B2" t="s">
-        <v>1613</v>
-      </c>
-      <c r="D2" s="57" t="s">
-        <v>1612</v>
-      </c>
+        <v>1607</v>
+      </c>
+      <c r="C2" t="s">
+        <v>1608</v>
+      </c>
+      <c r="D2" s="54"/>
       <c r="H2" t="s">
         <v>1446</v>
       </c>
@@ -6964,9 +7106,6 @@
       <formula1>"fixed-grid,dynamic-grid,pages,pages fixed-grid,pages dynamic-grid"</formula1>
     </dataValidation>
   </dataValidations>
-  <hyperlinks>
-    <hyperlink ref="D2" r:id="rId1" xr:uid="{DD120A9C-86CE-46FA-B0D0-DB0013007B2E}"/>
-  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="200" verticalDpi="200"/>
 </worksheet>
@@ -6990,10 +7129,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A1" s="55" t="s">
+      <c r="A1" s="56" t="s">
         <v>1329</v>
       </c>
-      <c r="B1" s="55"/>
+      <c r="B1" s="56"/>
       <c r="C1" s="16"/>
     </row>
     <row r="2" spans="1:3" ht="15.75" x14ac:dyDescent="0.25">
@@ -7018,10 +7157,10 @@
       </c>
     </row>
     <row r="6" spans="1:3" ht="60" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A6" s="54" t="s">
+      <c r="A6" s="55" t="s">
         <v>1324</v>
       </c>
-      <c r="B6" s="54"/>
+      <c r="B6" s="55"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -9278,7 +9417,7 @@
       <c r="C32" s="4" t="s">
         <v>1424</v>
       </c>
-      <c r="D32" s="56" t="s">
+      <c r="D32" s="57" t="s">
         <v>1483</v>
       </c>
     </row>
@@ -9289,7 +9428,7 @@
       <c r="C33" s="4" t="s">
         <v>1426</v>
       </c>
-      <c r="D33" s="56"/>
+      <c r="D33" s="57"/>
     </row>
     <row r="34" spans="2:4" x14ac:dyDescent="0.25">
       <c r="B34" s="31" t="s">
@@ -9309,7 +9448,7 @@
       <c r="C35" s="4" t="s">
         <v>1429</v>
       </c>
-      <c r="D35" s="56" t="s">
+      <c r="D35" s="57" t="s">
         <v>1482</v>
       </c>
     </row>
@@ -9320,7 +9459,7 @@
       <c r="C36" s="4" t="s">
         <v>1434</v>
       </c>
-      <c r="D36" s="56"/>
+      <c r="D36" s="57"/>
     </row>
     <row r="37" spans="2:4" ht="75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B37" s="31" t="s">
@@ -9329,7 +9468,7 @@
       <c r="C37" s="4" t="s">
         <v>1436</v>
       </c>
-      <c r="D37" s="56"/>
+      <c r="D37" s="57"/>
     </row>
     <row r="38" spans="2:4" ht="45" x14ac:dyDescent="0.25">
       <c r="B38" s="31" t="s">
@@ -9360,7 +9499,7 @@
       <c r="C40" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="D40" s="56" t="s">
+      <c r="D40" s="57" t="s">
         <v>1476</v>
       </c>
     </row>
@@ -9371,7 +9510,7 @@
       <c r="C41" s="4" t="s">
         <v>1288</v>
       </c>
-      <c r="D41" s="56"/>
+      <c r="D41" s="57"/>
     </row>
     <row r="42" spans="2:4" ht="90" x14ac:dyDescent="0.25">
       <c r="B42" s="31" t="s">

</xml_diff>